<commit_message>
hoàn thành báo cáo sử dụng điểm
</commit_message>
<xml_diff>
--- a/CMS/wwwroot/Templates/Excels/Reports/SummaryReportTemplate.xlsx
+++ b/CMS/wwwroot/Templates/Excels/Reports/SummaryReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vets\PRU-Gift\cms\CMS\wwwroot\Templates\Excels\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vets\dai-ichi-life\cms\CMS\wwwroot\Templates\Excels\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE91C2D-3F56-4AEF-B0CC-17405485ADB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A94C4-F004-4A2B-9024-7A41AFDD9D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD67CDD7-FCC7-4ADD-BAE1-721B997C6729}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>Hủy đơn hàng</t>
   </si>
   <si>
-    <t>Báo cáo tổng hợp</t>
-  </si>
-  <si>
     <t>{{item.Code}}</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>&lt;&lt;group mergelabels=merge2&gt;&gt;</t>
+  </si>
+  <si>
+    <t>{{Title}}</t>
   </si>
 </sst>
 </file>
@@ -290,13 +290,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -644,28 +644,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
+      <c r="A1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
     </row>
     <row r="2" spans="1:20" ht="21.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -676,16 +676,16 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="I2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -777,124 +777,124 @@
     </row>
     <row r="5" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="T5" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
+      <c r="B8" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>